<commit_message>
feat(templates): add Excel templates import and selector; add artifact kind; admin exports Soort column; add admin route; UI fixes (tooltips, responsive VRAAK, modal scroll)
</commit_message>
<xml_diff>
--- a/public/Jaarplanning-25-26.xlsx
+++ b/public/Jaarplanning-25-26.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hannl-my.sharepoint.com/personal/bastiaan_koekoek_han_nl/Documents/AI toepassingen bouwen/Jouw Portfolio plan maken/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkkbh\Documents\Curso-ai\Def-apps\Jouw Portfolio plan\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAB4D4D5-6060-42ED-B17B-A8725D0652CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD38CDD-6F4F-4F09-AF3E-EBF8617423A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F2EA1C8-8B22-4538-80E5-10DD06A62031}"/>
+    <workbookView xWindow="4032" yWindow="1692" windowWidth="17280" windowHeight="8880" xr2:uid="{1F2EA1C8-8B22-4538-80E5-10DD06A62031}"/>
   </bookViews>
   <sheets>
     <sheet name="Lesweekplanning" sheetId="1" r:id="rId1"/>
@@ -203,9 +203,6 @@
     <t>Jaar</t>
   </si>
   <si>
-    <t>0.0 nuweek</t>
-  </si>
-  <si>
     <t>0.1 nulwee</t>
   </si>
   <si>
@@ -345,6 +342,9 @@
   </si>
   <si>
     <t>Jaarafsluiting</t>
+  </si>
+  <si>
+    <t>0.0 nulweek</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
   <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -863,7 +863,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2">
         <v>45887</v>
@@ -874,7 +874,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2">
         <f>B2+7</f>
@@ -886,7 +886,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>45901</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5:B25" si="0">B4+7</f>
@@ -909,7 +909,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" si="0"/>
@@ -921,7 +921,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" si="0"/>
@@ -933,7 +933,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" si="0"/>
@@ -945,7 +945,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" si="0"/>
@@ -957,7 +957,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" si="0"/>
@@ -969,7 +969,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" si="0"/>
@@ -981,7 +981,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" si="0"/>
@@ -993,7 +993,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" si="0"/>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" si="0"/>
@@ -1017,7 +1017,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" si="0"/>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
         <f t="shared" si="0"/>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <f t="shared" si="0"/>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
         <f t="shared" si="0"/>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
         <f t="shared" si="0"/>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2">
         <f t="shared" si="0"/>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
         <f t="shared" si="0"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2">
         <f t="shared" si="0"/>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
         <f t="shared" si="0"/>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
         <f t="shared" si="0"/>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
         <f t="shared" si="0"/>
@@ -1149,12 +1149,12 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="2">
         <v>46055</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="2">
         <f t="shared" ref="B28:B49" si="1">B27+7</f>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5">
         <f t="shared" si="1"/>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="2">
         <f t="shared" si="1"/>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="2">
         <f t="shared" si="1"/>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="2">
         <f t="shared" si="1"/>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="2">
         <f t="shared" si="1"/>
@@ -1237,7 +1237,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" s="2">
         <f t="shared" si="1"/>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" s="2">
         <f t="shared" si="1"/>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="2">
         <f t="shared" si="1"/>
@@ -1273,7 +1273,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="2">
         <f t="shared" si="1"/>
@@ -1285,7 +1285,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" s="2">
         <f t="shared" si="1"/>
@@ -1297,7 +1297,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2">
         <f t="shared" si="1"/>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2">
         <f t="shared" si="1"/>
@@ -1321,7 +1321,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="2">
         <f t="shared" si="1"/>
@@ -1333,7 +1333,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" s="2">
         <f t="shared" si="1"/>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" s="2">
         <f t="shared" si="1"/>
@@ -1357,7 +1357,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="2">
         <f t="shared" si="1"/>
@@ -1369,7 +1369,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="2">
         <f t="shared" si="1"/>
@@ -1381,7 +1381,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B46" s="2">
         <f t="shared" si="1"/>
@@ -1393,7 +1393,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="2">
         <f t="shared" si="1"/>
@@ -1405,7 +1405,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="2">
         <f t="shared" si="1"/>
@@ -1417,7 +1417,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49" s="2">
         <f t="shared" si="1"/>

</xml_diff>